<commit_message>
08.05.19 Today Sales Info
</commit_message>
<xml_diff>
--- a/May/Othes/Allocation Sheet.xlsx
+++ b/May/Othes/Allocation Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
   <si>
     <t>BL60</t>
   </si>
@@ -205,9 +205,6 @@
     <t>D39</t>
   </si>
   <si>
-    <t>D52j</t>
-  </si>
-  <si>
     <t>D75</t>
   </si>
   <si>
@@ -319,7 +316,13 @@
     <t xml:space="preserve"> Date : </t>
   </si>
   <si>
-    <t>DSR NAME:</t>
+    <t>D52+</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>DSR NAME:      MD ROBIUL ISLAM</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -610,13 +613,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -710,23 +737,36 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -734,19 +774,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -761,12 +792,14 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1160,7 +1193,7 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="K4" sqref="K4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1180,62 +1213,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="32.25" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="54" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+    </row>
+    <row r="3" spans="1:16" s="35" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-    </row>
-    <row r="3" spans="1:16" s="52" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
     </row>
     <row r="4" spans="1:16" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
+      <c r="A4" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
@@ -1243,11 +1276,11 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
       <c r="J4" s="26"/>
-      <c r="K4" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="L4" s="50"/>
-      <c r="M4" s="51"/>
+      <c r="K4" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" s="52"/>
+      <c r="M4" s="53"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" thickTop="1">
       <c r="A5" s="11" t="s">
@@ -1266,7 +1299,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="11" t="s">
@@ -1301,7 +1334,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I6" s="4">
         <v>5750</v>
@@ -1360,7 +1393,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="7">
         <v>800</v>
@@ -1371,7 +1404,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" s="4">
         <v>7490</v>
@@ -1394,7 +1427,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I10" s="4">
         <v>8340</v>
@@ -1452,7 +1485,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="7">
         <v>910</v>
@@ -1486,7 +1519,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I14" s="4">
         <v>4690</v>
@@ -1509,7 +1542,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I15" s="4">
         <v>5390</v>
@@ -1544,7 +1577,7 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="7">
         <v>1010</v>
@@ -1647,7 +1680,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I21" s="4">
         <v>4080</v>
@@ -1670,7 +1703,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I22" s="4">
         <v>4080</v>
@@ -1716,7 +1749,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I24" s="4">
         <v>4640</v>
@@ -1751,10 +1784,10 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="B26" s="7">
-        <v>1290</v>
+        <v>1190</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1808,7 +1841,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I28" s="4">
         <v>5440</v>
@@ -1820,7 +1853,7 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="7">
         <v>1290</v>
@@ -1843,7 +1876,7 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="7">
         <v>1190</v>
@@ -1900,7 +1933,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I32" s="9">
         <v>12590</v>
@@ -1923,7 +1956,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I33" s="4">
         <v>12240</v>
@@ -1946,7 +1979,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I34" s="9">
         <v>12090</v>
@@ -1969,7 +2002,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I35" s="4">
         <v>10840</v>
@@ -1992,7 +2025,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I36" s="4">
         <v>12490</v>
@@ -2004,7 +2037,7 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="7">
         <v>1050</v>
@@ -2015,7 +2048,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I37" s="4">
         <v>12800</v>
@@ -2027,7 +2060,7 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="7">
         <v>1200</v>
@@ -2038,7 +2071,7 @@
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I38" s="4">
         <v>17790</v>
@@ -2061,7 +2094,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I39" s="4">
         <v>7740</v>
@@ -2083,8 +2116,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="9"/>
+      <c r="H40" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I40" s="9">
+        <v>5750</v>
+      </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
@@ -2092,7 +2129,7 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B41" s="7">
         <v>1330</v>
@@ -2159,18 +2196,18 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="46" t="s">
+      <c r="H44" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="47"/>
+      <c r="I44" s="45"/>
       <c r="J44" s="25"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="46"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
       <c r="M44" s="17"/>
     </row>
     <row r="45" spans="1:13" ht="15.75">
       <c r="A45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" s="7">
         <v>1460</v>
@@ -2180,16 +2217,16 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="46"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="40"/>
     </row>
     <row r="46" spans="1:13" ht="15.75">
       <c r="A46" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="7">
         <v>1470</v>
@@ -2199,18 +2236,18 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="44" t="s">
+      <c r="H46" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="44"/>
-      <c r="L46" s="44"/>
-      <c r="M46" s="43"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="54"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47" s="7">
         <v>1590</v>
@@ -2221,21 +2258,21 @@
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J47" s="45" t="s">
+      <c r="J47" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="43"/>
+      <c r="K47" s="42"/>
+      <c r="L47" s="42"/>
+      <c r="M47" s="55"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="7">
         <v>1480</v>
@@ -2252,7 +2289,7 @@
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
-      <c r="M48" s="43"/>
+      <c r="M48" s="55"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="2" t="s">
@@ -2273,7 +2310,7 @@
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
-      <c r="M49" s="43"/>
+      <c r="M49" s="55"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="3" t="s">
@@ -2294,7 +2331,7 @@
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
-      <c r="M50" s="43"/>
+      <c r="M50" s="55"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="3" t="s">
@@ -2315,7 +2352,7 @@
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
-      <c r="M51" s="43"/>
+      <c r="M51" s="55"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="3" t="s">
@@ -2336,7 +2373,7 @@
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
-      <c r="M52" s="43"/>
+      <c r="M52" s="55"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="3" t="s">
@@ -2357,7 +2394,7 @@
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
-      <c r="M53" s="43"/>
+      <c r="M53" s="55"/>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="3" t="s">
@@ -2378,7 +2415,7 @@
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
-      <c r="M54" s="43"/>
+      <c r="M54" s="55"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="3" t="s">
@@ -2399,7 +2436,7 @@
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
-      <c r="M55" s="43"/>
+      <c r="M55" s="55"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="2" t="s">
@@ -2420,7 +2457,7 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
-      <c r="M56" s="43"/>
+      <c r="M56" s="56"/>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="15"/>
@@ -2438,11 +2475,11 @@
       <c r="M57" s="27"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
+      <c r="A58" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
       <c r="D58" s="32"/>
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
@@ -2451,15 +2488,15 @@
       <c r="I58" s="33"/>
       <c r="J58" s="31"/>
       <c r="K58" s="32"/>
-      <c r="L58" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="M58" s="35"/>
+      <c r="L58" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="M58" s="44"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="40"/>
-      <c r="B59" s="40"/>
-      <c r="C59" s="40"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -2472,9 +2509,9 @@
       <c r="M59" s="37"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="40"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
+      <c r="A60" s="36"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -2487,11 +2524,11 @@
       <c r="M60" s="37"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
+      <c r="A61" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
       <c r="D61" s="29"/>
       <c r="E61" s="29"/>
       <c r="F61" s="29"/>
@@ -2500,8 +2537,8 @@
       <c r="I61" s="30"/>
       <c r="J61" s="29"/>
       <c r="K61" s="28"/>
-      <c r="L61" s="36"/>
-      <c r="M61" s="36"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>

<commit_message>
13.05.19 Today Sales Updated
</commit_message>
<xml_diff>
--- a/May/Othes/Allocation Sheet.xlsx
+++ b/May/Othes/Allocation Sheet.xlsx
@@ -322,7 +322,7 @@
     <t>R40</t>
   </si>
   <si>
-    <t>DSR NAME:      MD ROBIUL ISLAM</t>
+    <t>DSR NAME:      MD SHOHEL RANA</t>
   </si>
 </sst>
 </file>
@@ -738,6 +738,36 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -750,12 +780,18 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -764,42 +800,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1193,7 +1193,7 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:M4"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1213,62 +1213,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="32.25" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
     </row>
     <row r="3" spans="1:16" s="35" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="1:16" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
@@ -1276,11 +1276,11 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
       <c r="J4" s="26"/>
-      <c r="K4" s="51" t="s">
+      <c r="K4" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="L4" s="52"/>
-      <c r="M4" s="53"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" thickTop="1">
       <c r="A5" s="11" t="s">
@@ -2196,13 +2196,13 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40" t="s">
+      <c r="H44" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="45"/>
+      <c r="I44" s="37"/>
       <c r="J44" s="25"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="36"/>
       <c r="M44" s="17"/>
     </row>
     <row r="45" spans="1:13" ht="15.75">
@@ -2217,12 +2217,12 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="40"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
     </row>
     <row r="46" spans="1:13" ht="15.75">
       <c r="A46" s="2" t="s">
@@ -2236,14 +2236,14 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="54"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="51"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="2" t="s">
@@ -2263,12 +2263,12 @@
       <c r="I47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J47" s="42" t="s">
+      <c r="J47" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="K47" s="42"/>
-      <c r="L47" s="42"/>
-      <c r="M47" s="55"/>
+      <c r="K47" s="54"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="52"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="2" t="s">
@@ -2289,7 +2289,7 @@
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
-      <c r="M48" s="55"/>
+      <c r="M48" s="52"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="2" t="s">
@@ -2310,7 +2310,7 @@
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
-      <c r="M49" s="55"/>
+      <c r="M49" s="52"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="3" t="s">
@@ -2331,7 +2331,7 @@
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
-      <c r="M50" s="55"/>
+      <c r="M50" s="52"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="3" t="s">
@@ -2352,7 +2352,7 @@
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
-      <c r="M51" s="55"/>
+      <c r="M51" s="52"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="3" t="s">
@@ -2373,7 +2373,7 @@
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
-      <c r="M52" s="55"/>
+      <c r="M52" s="52"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="3" t="s">
@@ -2394,7 +2394,7 @@
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
-      <c r="M53" s="55"/>
+      <c r="M53" s="52"/>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="3" t="s">
@@ -2415,7 +2415,7 @@
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
-      <c r="M54" s="55"/>
+      <c r="M54" s="52"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="3" t="s">
@@ -2436,7 +2436,7 @@
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
-      <c r="M55" s="55"/>
+      <c r="M55" s="52"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="2" t="s">
@@ -2457,7 +2457,7 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
-      <c r="M56" s="56"/>
+      <c r="M56" s="53"/>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="15"/>
@@ -2475,11 +2475,11 @@
       <c r="M57" s="27"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="43"/>
-      <c r="C58" s="43"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="55"/>
       <c r="D58" s="32"/>
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
@@ -2488,15 +2488,15 @@
       <c r="I58" s="33"/>
       <c r="J58" s="31"/>
       <c r="K58" s="32"/>
-      <c r="L58" s="44" t="s">
+      <c r="L58" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="M58" s="44"/>
+      <c r="M58" s="56"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
+      <c r="A59" s="46"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="46"/>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -2505,13 +2505,13 @@
       <c r="I59" s="16"/>
       <c r="J59" s="23"/>
       <c r="K59" s="14"/>
-      <c r="L59" s="37"/>
-      <c r="M59" s="37"/>
+      <c r="L59" s="47"/>
+      <c r="M59" s="47"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
+      <c r="A60" s="46"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="46"/>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -2520,15 +2520,15 @@
       <c r="I60" s="16"/>
       <c r="J60" s="23"/>
       <c r="K60" s="14"/>
-      <c r="L60" s="37"/>
-      <c r="M60" s="37"/>
+      <c r="L60" s="47"/>
+      <c r="M60" s="47"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="38" t="s">
+      <c r="A61" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="48"/>
       <c r="D61" s="29"/>
       <c r="E61" s="29"/>
       <c r="F61" s="29"/>
@@ -2537,18 +2537,11 @@
       <c r="I61" s="30"/>
       <c r="J61" s="29"/>
       <c r="K61" s="28"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="39"/>
+      <c r="L61" s="49"/>
+      <c r="M61" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="K4:M4"/>
     <mergeCell ref="A59:C60"/>
     <mergeCell ref="L59:M60"/>
     <mergeCell ref="A61:C61"/>
@@ -2559,6 +2552,13 @@
     <mergeCell ref="J47:L47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="L58:M58"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
19.05.19 Today Morning Sales Updated
</commit_message>
<xml_diff>
--- a/May/Othes/Allocation Sheet.xlsx
+++ b/May/Othes/Allocation Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
   <si>
     <t>BL60</t>
   </si>
@@ -322,7 +322,10 @@
     <t>R40</t>
   </si>
   <si>
-    <t>DSR NAME:      MD SHOHEL RANA</t>
+    <t>D54+</t>
+  </si>
+  <si>
+    <t>DSR NAME:   MD SHOHEL RANA</t>
   </si>
 </sst>
 </file>
@@ -738,9 +741,42 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -767,39 +803,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1192,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection sqref="A1:M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1213,62 +1216,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="32.25" customHeight="1">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
     </row>
     <row r="3" spans="1:16" s="35" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
     </row>
     <row r="4" spans="1:16" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
@@ -1276,11 +1279,11 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
       <c r="J4" s="26"/>
-      <c r="K4" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="L4" s="44"/>
-      <c r="M4" s="45"/>
+      <c r="K4" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" s="55"/>
+      <c r="M4" s="56"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" thickTop="1">
       <c r="A5" s="11" t="s">
@@ -1522,7 +1525,7 @@
         <v>87</v>
       </c>
       <c r="I14" s="4">
-        <v>4690</v>
+        <v>4500</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1669,10 +1672,10 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="2" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="B21" s="7">
-        <v>995</v>
+        <v>1170</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1702,12 +1705,8 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I22" s="4">
-        <v>4080</v>
-      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="4"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
@@ -1729,7 +1728,7 @@
         <v>39</v>
       </c>
       <c r="I23" s="4">
-        <v>4360</v>
+        <v>4220</v>
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
@@ -1844,7 +1843,7 @@
         <v>67</v>
       </c>
       <c r="I28" s="4">
-        <v>5440</v>
+        <v>5100</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
@@ -2051,7 +2050,7 @@
         <v>82</v>
       </c>
       <c r="I37" s="4">
-        <v>12800</v>
+        <v>10330</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -2196,13 +2195,13 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36" t="s">
+      <c r="H44" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="37"/>
+      <c r="I44" s="48"/>
       <c r="J44" s="25"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
       <c r="M44" s="17"/>
     </row>
     <row r="45" spans="1:13" ht="15.75">
@@ -2217,12 +2216,12 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="36"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="40"/>
     </row>
     <row r="46" spans="1:13" ht="15.75">
       <c r="A46" s="2" t="s">
@@ -2236,14 +2235,14 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-      <c r="L46" s="50"/>
-      <c r="M46" s="51"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="42"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="2" t="s">
@@ -2263,12 +2262,12 @@
       <c r="I47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J47" s="54" t="s">
+      <c r="J47" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="K47" s="54"/>
-      <c r="L47" s="54"/>
-      <c r="M47" s="52"/>
+      <c r="K47" s="45"/>
+      <c r="L47" s="45"/>
+      <c r="M47" s="43"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="2" t="s">
@@ -2289,7 +2288,7 @@
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
-      <c r="M48" s="52"/>
+      <c r="M48" s="43"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="2" t="s">
@@ -2310,7 +2309,7 @@
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
-      <c r="M49" s="52"/>
+      <c r="M49" s="43"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="3" t="s">
@@ -2331,7 +2330,7 @@
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
-      <c r="M50" s="52"/>
+      <c r="M50" s="43"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="3" t="s">
@@ -2352,7 +2351,7 @@
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
-      <c r="M51" s="52"/>
+      <c r="M51" s="43"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="3" t="s">
@@ -2373,7 +2372,7 @@
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
-      <c r="M52" s="52"/>
+      <c r="M52" s="43"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="3" t="s">
@@ -2394,7 +2393,7 @@
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
-      <c r="M53" s="52"/>
+      <c r="M53" s="43"/>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="3" t="s">
@@ -2415,14 +2414,14 @@
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
-      <c r="M54" s="52"/>
+      <c r="M54" s="43"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B55" s="3">
-        <v>6210</v>
+        <v>5290</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
@@ -2436,7 +2435,7 @@
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
-      <c r="M55" s="52"/>
+      <c r="M55" s="43"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="2" t="s">
@@ -2457,7 +2456,7 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
-      <c r="M56" s="53"/>
+      <c r="M56" s="44"/>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="15"/>
@@ -2475,11 +2474,11 @@
       <c r="M57" s="27"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="55"/>
-      <c r="C58" s="55"/>
+      <c r="B58" s="46"/>
+      <c r="C58" s="46"/>
       <c r="D58" s="32"/>
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
@@ -2488,15 +2487,15 @@
       <c r="I58" s="33"/>
       <c r="J58" s="31"/>
       <c r="K58" s="32"/>
-      <c r="L58" s="56" t="s">
+      <c r="L58" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="M58" s="56"/>
+      <c r="M58" s="47"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="46"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="46"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -2505,13 +2504,13 @@
       <c r="I59" s="16"/>
       <c r="J59" s="23"/>
       <c r="K59" s="14"/>
-      <c r="L59" s="47"/>
-      <c r="M59" s="47"/>
+      <c r="L59" s="37"/>
+      <c r="M59" s="37"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="46"/>
-      <c r="B60" s="46"/>
-      <c r="C60" s="46"/>
+      <c r="A60" s="36"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -2520,15 +2519,15 @@
       <c r="I60" s="16"/>
       <c r="J60" s="23"/>
       <c r="K60" s="14"/>
-      <c r="L60" s="47"/>
-      <c r="M60" s="47"/>
+      <c r="L60" s="37"/>
+      <c r="M60" s="37"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="48" t="s">
+      <c r="A61" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="48"/>
-      <c r="C61" s="48"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
       <c r="D61" s="29"/>
       <c r="E61" s="29"/>
       <c r="F61" s="29"/>
@@ -2537,11 +2536,18 @@
       <c r="I61" s="30"/>
       <c r="J61" s="29"/>
       <c r="K61" s="28"/>
-      <c r="L61" s="49"/>
-      <c r="M61" s="49"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="K4:M4"/>
     <mergeCell ref="A59:C60"/>
     <mergeCell ref="L59:M60"/>
     <mergeCell ref="A61:C61"/>
@@ -2552,13 +2558,6 @@
     <mergeCell ref="J47:L47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="L58:M58"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
20.05.19 Today morning Sales Updated
</commit_message>
<xml_diff>
--- a/May/Othes/Allocation Sheet.xlsx
+++ b/May/Othes/Allocation Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
   <si>
     <t>BL60</t>
   </si>
@@ -31,27 +31,18 @@
     <t>BL90</t>
   </si>
   <si>
-    <t>i10+</t>
-  </si>
-  <si>
     <t>D10</t>
   </si>
   <si>
     <t>L55</t>
   </si>
   <si>
-    <t>i60</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
     <t>Return</t>
   </si>
   <si>
-    <t xml:space="preserve">Issue </t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -133,9 +124,6 @@
     <t>V145</t>
   </si>
   <si>
-    <t>V98</t>
-  </si>
-  <si>
     <t>L40</t>
   </si>
   <si>
@@ -160,12 +148,6 @@
     <t>B17i</t>
   </si>
   <si>
-    <t>V48</t>
-  </si>
-  <si>
-    <t>i75</t>
-  </si>
-  <si>
     <t>i90</t>
   </si>
   <si>
@@ -175,9 +157,6 @@
     <t>D40</t>
   </si>
   <si>
-    <t>T110</t>
-  </si>
-  <si>
     <t>T140</t>
   </si>
   <si>
@@ -202,15 +181,9 @@
     <t>D38</t>
   </si>
   <si>
-    <t>D39</t>
-  </si>
-  <si>
     <t>D75</t>
   </si>
   <si>
-    <t>D91</t>
-  </si>
-  <si>
     <t>i95</t>
   </si>
   <si>
@@ -226,21 +199,12 @@
     <t>BL70</t>
   </si>
   <si>
-    <t>BL100</t>
-  </si>
-  <si>
-    <t>L65</t>
-  </si>
-  <si>
     <t>L120</t>
   </si>
   <si>
     <t>L150</t>
   </si>
   <si>
-    <t>T85</t>
-  </si>
-  <si>
     <t>V75m</t>
   </si>
   <si>
@@ -262,24 +226,9 @@
     <t>P9+</t>
   </si>
   <si>
-    <t>S5Helio</t>
-  </si>
-  <si>
-    <t>S10Helio</t>
-  </si>
-  <si>
-    <t>SymTab25</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>i110_SKD</t>
-  </si>
-  <si>
-    <t>V75 SKD</t>
-  </si>
-  <si>
     <t>Received By</t>
   </si>
   <si>
@@ -292,9 +241,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>v128</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tulip-2 </t>
   </si>
   <si>
@@ -325,7 +271,64 @@
     <t>D54+</t>
   </si>
   <si>
-    <t>DSR NAME:   MD SHOHEL RANA</t>
+    <t>BL20</t>
+  </si>
+  <si>
+    <t>D52j</t>
+  </si>
+  <si>
+    <t>L100</t>
+  </si>
+  <si>
+    <t>L300</t>
+  </si>
+  <si>
+    <t>i10+skd</t>
+  </si>
+  <si>
+    <t>i110skd</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>V120</t>
+  </si>
+  <si>
+    <t>V128</t>
+  </si>
+  <si>
+    <t>V42</t>
+  </si>
+  <si>
+    <t>V48_SKD</t>
+  </si>
+  <si>
+    <t>V75m_2GB</t>
+  </si>
+  <si>
+    <t>V75skd</t>
+  </si>
+  <si>
+    <t>V90</t>
+  </si>
+  <si>
+    <t>V98skd</t>
+  </si>
+  <si>
+    <t>P8 Pro</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>DSR NAME:   Md Shohel Rana</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -556,58 +559,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -646,7 +597,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -720,7 +671,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -750,19 +701,49 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -777,32 +758,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -825,7 +788,7 @@
       <xdr:rowOff>9719</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>38878</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>9720</xdr:rowOff>
@@ -863,13 +826,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>194388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>9719</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>194390</xdr:rowOff>
@@ -1193,1371 +1156,1667 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection sqref="A1:M61"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="N61" sqref="A1:O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="3.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="3" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="12" width="7.140625" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="32.25" customHeight="1">
-      <c r="A1" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-    </row>
-    <row r="3" spans="1:16" s="35" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-    </row>
-    <row r="4" spans="1:16" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="53" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+    <row r="1" spans="1:18" ht="32.25" customHeight="1">
+      <c r="A1" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+    </row>
+    <row r="3" spans="1:18" s="35" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+    </row>
+    <row r="4" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A4" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="54" t="s">
+      <c r="J4" s="22"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickTop="1">
+      <c r="A5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="L4" s="55"/>
-      <c r="M4" s="56"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" thickTop="1">
-      <c r="A5" s="11" t="s">
+      <c r="D5" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+    </row>
+    <row r="6" spans="1:18" ht="15.95" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B6" s="7">
         <v>800</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6">
+        <v>875</v>
+      </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="I6" s="4">
-        <v>5750</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7490</v>
+      </c>
+      <c r="K6" s="6">
+        <v>7990</v>
+      </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" ht="15.75">
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.95" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="7">
         <v>865</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6">
+        <v>925</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="9">
-        <v>7910</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="9">
+        <v>9190</v>
+      </c>
+      <c r="K7" s="6">
+        <v>9990</v>
+      </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="P7" s="34"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="R7" s="34"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.95" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B8" s="7">
         <v>810</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>880</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="2">
-        <v>7890</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5750</v>
+      </c>
+      <c r="K8" s="6">
+        <v>6190</v>
+      </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.95" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B9" s="7">
         <v>800</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>870</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="4">
-        <v>7490</v>
-      </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="4">
+        <v>17790</v>
+      </c>
+      <c r="K9" s="6">
+        <v>18990</v>
+      </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.95" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="7">
         <v>795</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6">
+        <v>865</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="4">
-        <v>8340</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="4">
+        <v>10330</v>
+      </c>
+      <c r="K10" s="6">
+        <v>10990</v>
+      </c>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.95" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" s="7">
         <v>790</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6">
+        <v>860</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="4">
-        <v>9190</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5570</v>
+      </c>
+      <c r="K11" s="6">
+        <v>5990</v>
+      </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:18" ht="15.95" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B12" s="7">
-        <v>915</v>
-      </c>
-      <c r="C12" s="6"/>
+        <v>970</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1060</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="4">
-        <v>3560</v>
-      </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J12" s="4">
+        <v>4640</v>
+      </c>
+      <c r="K12" s="6">
+        <v>4990</v>
+      </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.95" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B13" s="7">
-        <v>910</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>900</v>
+      </c>
+      <c r="C13" s="6">
+        <v>975</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="4">
-        <v>3340</v>
-      </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="4">
+        <v>5650</v>
+      </c>
+      <c r="K13" s="6">
+        <v>6150</v>
+      </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:18" ht="15.95" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B14" s="7">
-        <v>890</v>
-      </c>
-      <c r="C14" s="6"/>
+        <v>915</v>
+      </c>
+      <c r="C14" s="6">
+        <v>990</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I14" s="4">
-        <v>4500</v>
-      </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="4">
+        <v>5020</v>
+      </c>
+      <c r="K14" s="6">
+        <v>5390</v>
+      </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.95" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="B15" s="7">
-        <v>920</v>
-      </c>
-      <c r="C15" s="6"/>
+        <v>910</v>
+      </c>
+      <c r="C15" s="6">
+        <v>980</v>
+      </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="I15" s="4">
-        <v>5390</v>
-      </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="4">
+        <v>5280</v>
+      </c>
+      <c r="K15" s="6">
+        <v>5690</v>
+      </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.95" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B16" s="7">
-        <v>880</v>
-      </c>
-      <c r="C16" s="6"/>
+        <v>890</v>
+      </c>
+      <c r="C16" s="6">
+        <v>970</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="6"/>
+      <c r="I16" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="4">
-        <v>4970</v>
-      </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="J16" s="4">
+        <v>5100</v>
+      </c>
+      <c r="K16" s="6">
+        <v>5490</v>
+      </c>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.95" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="B17" s="7">
-        <v>1010</v>
-      </c>
-      <c r="C17" s="6"/>
+        <v>920</v>
+      </c>
+      <c r="C17" s="6">
+        <v>999</v>
+      </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="4">
-        <v>3710</v>
-      </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="4">
+        <v>5560</v>
+      </c>
+      <c r="K17" s="6">
+        <v>5990</v>
+      </c>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.95" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B18" s="7">
-        <v>970</v>
-      </c>
-      <c r="C18" s="6"/>
+        <v>880</v>
+      </c>
+      <c r="C18" s="6">
+        <v>950</v>
+      </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" s="4">
-        <v>3620</v>
-      </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="4">
+        <v>6090</v>
+      </c>
+      <c r="K18" s="6">
+        <v>6590</v>
+      </c>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.95" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="7">
         <v>1000</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="6">
+        <v>1090</v>
+      </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="4">
-        <v>4620</v>
-      </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5390</v>
+      </c>
+      <c r="K19" s="6">
+        <v>5790</v>
+      </c>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.95" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="7">
         <v>995</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="6">
+        <v>1075</v>
+      </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="4">
-        <v>4520</v>
-      </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" s="4">
+        <v>3630</v>
+      </c>
+      <c r="K20" s="6">
+        <v>3890</v>
+      </c>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.95" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="B21" s="7">
-        <v>1170</v>
-      </c>
-      <c r="C21" s="6"/>
+        <v>1000</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1090</v>
+      </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="4">
-        <v>4080</v>
-      </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="4">
+        <v>3560</v>
+      </c>
+      <c r="K21" s="6">
+        <v>3840</v>
+      </c>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.95" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B22" s="7">
-        <v>1000</v>
-      </c>
-      <c r="C22" s="6"/>
+        <v>960</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1040</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="4">
+        <v>3340</v>
+      </c>
+      <c r="K22" s="6">
+        <v>3590</v>
+      </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.95" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B23" s="7">
-        <v>960</v>
-      </c>
-      <c r="C23" s="6"/>
+        <v>1040</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1120</v>
+      </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="4">
-        <v>4220</v>
-      </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="4">
+        <v>5390</v>
+      </c>
+      <c r="K23" s="6">
+        <v>5790</v>
+      </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.95" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B24" s="7">
-        <v>980</v>
-      </c>
-      <c r="C24" s="6"/>
+        <v>1290</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1390</v>
+      </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I24" s="4">
-        <v>4640</v>
-      </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" s="4">
+        <v>5740</v>
+      </c>
+      <c r="K24" s="6">
+        <v>6190</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.95" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B25" s="7">
-        <v>1040</v>
-      </c>
-      <c r="C25" s="6"/>
+        <v>1190</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1290</v>
+      </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="4">
-        <v>5650</v>
-      </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25" s="4">
+        <v>4500</v>
+      </c>
+      <c r="K25" s="6">
+        <v>4790</v>
+      </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.95" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="B26" s="7">
-        <v>1190</v>
-      </c>
-      <c r="C26" s="6"/>
+        <v>1270</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1370</v>
+      </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" s="4">
-        <v>5020</v>
-      </c>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="4">
+        <v>4970</v>
+      </c>
+      <c r="K26" s="6">
+        <v>5290</v>
+      </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.95" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B27" s="7">
+        <v>1170</v>
+      </c>
+      <c r="C27" s="6">
         <v>1270</v>
       </c>
-      <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="4">
-        <v>5280</v>
-      </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J27" s="4">
+        <v>4015</v>
+      </c>
+      <c r="K27" s="6">
+        <v>4390</v>
+      </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.95" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B28" s="7">
         <v>1190</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="6">
+        <v>1290</v>
+      </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" s="4">
-        <v>5100</v>
-      </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="4">
+        <v>3710</v>
+      </c>
+      <c r="K28" s="6">
+        <v>3890</v>
+      </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.95" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B29" s="7">
         <v>1290</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="6">
+        <v>1390</v>
+      </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="I29" s="4">
-        <v>5560</v>
-      </c>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29" s="4">
+        <v>3620</v>
+      </c>
+      <c r="K29" s="6">
+        <v>4290</v>
+      </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.95" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B30" s="7">
-        <v>1190</v>
-      </c>
-      <c r="C30" s="6"/>
+        <v>1225</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1325</v>
+      </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I30" s="9">
-        <v>6090</v>
-      </c>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="9">
+        <v>4620</v>
+      </c>
+      <c r="K30" s="6">
+        <v>4999</v>
+      </c>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="1:15" ht="15.95" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B31" s="7">
-        <v>1080</v>
-      </c>
-      <c r="C31" s="6"/>
+        <v>1220</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1320</v>
+      </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I31" s="9">
-        <v>5390</v>
-      </c>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="9">
+        <v>4520</v>
+      </c>
+      <c r="K31" s="6">
+        <v>4899</v>
+      </c>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.95" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B32" s="7">
-        <v>1100</v>
-      </c>
-      <c r="C32" s="6"/>
+        <v>1460</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1590</v>
+      </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="I32" s="9">
-        <v>12590</v>
-      </c>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="J32" s="9">
+        <v>4080</v>
+      </c>
+      <c r="K32" s="6">
+        <v>4390</v>
+      </c>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.95" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="B33" s="7">
-        <v>1120</v>
-      </c>
-      <c r="C33" s="6"/>
+        <v>1470</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1590</v>
+      </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="I33" s="4">
-        <v>12240</v>
-      </c>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="J33" s="4">
+        <v>4220</v>
+      </c>
+      <c r="K33" s="6">
+        <v>4540</v>
+      </c>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="1:15" ht="15.95" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B34" s="7">
-        <v>1040</v>
-      </c>
-      <c r="C34" s="6"/>
+        <v>1590</v>
+      </c>
+      <c r="C34" s="6">
+        <v>1740</v>
+      </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I34" s="9">
-        <v>12090</v>
-      </c>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J34" s="9">
+        <v>12590</v>
+      </c>
+      <c r="K34" s="6">
+        <v>13490</v>
+      </c>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+    </row>
+    <row r="35" spans="1:15" ht="15.95" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="B35" s="7">
-        <v>1100</v>
-      </c>
-      <c r="C35" s="6"/>
+        <v>1080</v>
+      </c>
+      <c r="C35" s="6">
+        <v>1160</v>
+      </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="I35" s="4">
-        <v>10840</v>
-      </c>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" s="4">
+        <v>12240</v>
+      </c>
+      <c r="K35" s="6">
+        <v>12990</v>
+      </c>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+    </row>
+    <row r="36" spans="1:15" ht="15.95" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B36" s="8">
         <v>1100</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="6">
+        <v>1199</v>
+      </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
-      <c r="H36" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="I36" s="4">
-        <v>12490</v>
-      </c>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="J36" s="4">
+        <v>8270</v>
+      </c>
+      <c r="K36" s="6">
+        <v>8990</v>
+      </c>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+    </row>
+    <row r="37" spans="1:15" ht="15.95" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B37" s="7">
-        <v>1050</v>
-      </c>
-      <c r="C37" s="6"/>
+        <v>1200</v>
+      </c>
+      <c r="C37" s="6">
+        <v>1290</v>
+      </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="I37" s="4">
-        <v>10330</v>
-      </c>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J37" s="4">
+        <v>12090</v>
+      </c>
+      <c r="K37" s="6">
+        <v>12990</v>
+      </c>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="1:15" ht="15.95" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="B38" s="7">
-        <v>1200</v>
-      </c>
-      <c r="C38" s="6"/>
+        <v>1120</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1220</v>
+      </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="I38" s="4">
-        <v>17790</v>
-      </c>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="J38" s="4">
+        <v>10840</v>
+      </c>
+      <c r="K38" s="6">
+        <v>11990</v>
+      </c>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+    </row>
+    <row r="39" spans="1:15" ht="15.95" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B39" s="7">
-        <v>1130</v>
-      </c>
-      <c r="C39" s="6"/>
+        <v>1730</v>
+      </c>
+      <c r="C39" s="6">
+        <v>1890</v>
+      </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="I39" s="4">
-        <v>7740</v>
-      </c>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J39" s="4">
+        <v>12490</v>
+      </c>
+      <c r="K39" s="6">
+        <v>13490</v>
+      </c>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="1:15" ht="15.95" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="7">
-        <v>1100</v>
-      </c>
-      <c r="C40" s="6"/>
+        <v>1040</v>
+      </c>
+      <c r="C40" s="6">
+        <v>1130</v>
+      </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="I40" s="9">
-        <v>5750</v>
-      </c>
-      <c r="J40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="9"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="1:15" ht="15.95" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B41" s="7">
-        <v>1330</v>
-      </c>
-      <c r="C41" s="6"/>
+        <v>1100</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1199</v>
+      </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="4"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="1:15" ht="15.95" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B42" s="7">
-        <v>1330</v>
-      </c>
-      <c r="C42" s="6"/>
+        <v>1100</v>
+      </c>
+      <c r="C42" s="6">
+        <v>1199</v>
+      </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="4"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="1:15" ht="15.95" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B43" s="7">
-        <v>1200</v>
-      </c>
-      <c r="C43" s="6"/>
+        <v>1050</v>
+      </c>
+      <c r="C43" s="6">
+        <v>1130</v>
+      </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="4"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
-    </row>
-    <row r="44" spans="1:13" ht="15.75">
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+    </row>
+    <row r="44" spans="1:15" ht="15.95" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B44" s="7">
-        <v>1220</v>
-      </c>
-      <c r="C44" s="6"/>
+        <v>1130</v>
+      </c>
+      <c r="C44" s="6">
+        <v>1230</v>
+      </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="I44" s="48"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="17"/>
-    </row>
-    <row r="45" spans="1:13" ht="15.75">
+      <c r="H44" s="6"/>
+      <c r="I44" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="42"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="17"/>
+    </row>
+    <row r="45" spans="1:15" ht="15.95" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="B45" s="7">
-        <v>1460</v>
-      </c>
-      <c r="C45" s="6"/>
+        <v>1100</v>
+      </c>
+      <c r="C45" s="6">
+        <v>1190</v>
+      </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="40"/>
-    </row>
-    <row r="46" spans="1:13" ht="15.75">
+      <c r="H45" s="6"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="41"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
+      <c r="O45" s="41"/>
+    </row>
+    <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B46" s="7">
-        <v>1470</v>
-      </c>
-      <c r="C46" s="6"/>
+        <v>1330</v>
+      </c>
+      <c r="C46" s="6">
+        <v>1450</v>
+      </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="42"/>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="H46" s="6"/>
+      <c r="I46" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
+      <c r="M46" s="51"/>
+      <c r="N46" s="51"/>
+      <c r="O46" s="52"/>
+    </row>
+    <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B47" s="7">
-        <v>1590</v>
-      </c>
-      <c r="C47" s="6"/>
+        <v>1200</v>
+      </c>
+      <c r="C47" s="6">
+        <v>1299</v>
+      </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J47" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="43"/>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="H47" s="6"/>
+      <c r="I47" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K47" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="L47" s="55"/>
+      <c r="M47" s="55"/>
+      <c r="N47" s="55"/>
+      <c r="O47" s="53"/>
+    </row>
+    <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="B48" s="7">
-        <v>1480</v>
-      </c>
-      <c r="C48" s="6"/>
+        <v>1250</v>
+      </c>
+      <c r="C48" s="6">
+        <v>1350</v>
+      </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="20">
+      <c r="H48" s="6"/>
+      <c r="I48" s="20">
         <v>1000</v>
       </c>
-      <c r="I48" s="21"/>
-      <c r="J48" s="6"/>
+      <c r="J48" s="21"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
-      <c r="M48" s="43"/>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="53"/>
+    </row>
+    <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B49" s="7">
-        <v>1730</v>
-      </c>
-      <c r="C49" s="6"/>
+        <v>1370</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1470</v>
+      </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="20">
+      <c r="H49" s="6"/>
+      <c r="I49" s="20">
         <v>500</v>
       </c>
-      <c r="I49" s="21"/>
-      <c r="J49" s="6"/>
+      <c r="J49" s="21"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
-      <c r="M49" s="43"/>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="53"/>
+    </row>
+    <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B50" s="3">
-        <v>1250</v>
-      </c>
-      <c r="C50" s="6"/>
+        <v>1890</v>
+      </c>
+      <c r="C50" s="6">
+        <v>2090</v>
+      </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="20">
+      <c r="H50" s="6"/>
+      <c r="I50" s="20">
         <v>100</v>
       </c>
-      <c r="I50" s="21"/>
-      <c r="J50" s="6"/>
+      <c r="J50" s="21"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
-      <c r="M50" s="43"/>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="53"/>
+    </row>
+    <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B51" s="3">
-        <v>1370</v>
-      </c>
-      <c r="C51" s="6"/>
+        <v>2780</v>
+      </c>
+      <c r="C51" s="6">
+        <v>2990</v>
+      </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="20">
+      <c r="H51" s="6"/>
+      <c r="I51" s="20">
         <v>50</v>
       </c>
-      <c r="I51" s="21"/>
-      <c r="J51" s="6"/>
+      <c r="J51" s="21"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
-      <c r="M51" s="43"/>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="53"/>
+    </row>
+    <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B52" s="3">
-        <v>1890</v>
-      </c>
-      <c r="C52" s="6"/>
+        <v>5290</v>
+      </c>
+      <c r="C52" s="6">
+        <v>5690</v>
+      </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
-      <c r="H52" s="20">
+      <c r="H52" s="6"/>
+      <c r="I52" s="20">
         <v>20</v>
       </c>
-      <c r="I52" s="21"/>
-      <c r="J52" s="6"/>
+      <c r="J52" s="21"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
-      <c r="M52" s="43"/>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="53"/>
+    </row>
+    <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B53" s="3">
-        <v>2780</v>
-      </c>
-      <c r="C53" s="6"/>
+        <v>5750</v>
+      </c>
+      <c r="C53" s="6">
+        <v>6190</v>
+      </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
-      <c r="H53" s="20">
+      <c r="H53" s="6"/>
+      <c r="I53" s="20">
         <v>10</v>
       </c>
-      <c r="I53" s="21"/>
-      <c r="J53" s="6"/>
+      <c r="J53" s="21"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
-      <c r="M53" s="43"/>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="53"/>
+    </row>
+    <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="B54" s="3">
         <v>6540</v>
       </c>
-      <c r="C54" s="6"/>
+      <c r="C54" s="6">
+        <v>6990</v>
+      </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
-      <c r="H54" s="20">
+      <c r="H54" s="6"/>
+      <c r="I54" s="20">
         <v>5</v>
       </c>
-      <c r="I54" s="21"/>
-      <c r="J54" s="6"/>
+      <c r="J54" s="21"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
-      <c r="M54" s="43"/>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="53"/>
+    </row>
+    <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B55" s="3">
-        <v>5290</v>
-      </c>
-      <c r="C55" s="6"/>
+        <v>8340</v>
+      </c>
+      <c r="C55" s="6">
+        <v>8990</v>
+      </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
-      <c r="H55" s="20">
+      <c r="H55" s="6"/>
+      <c r="I55" s="20">
         <v>2</v>
       </c>
-      <c r="I55" s="21"/>
-      <c r="J55" s="6"/>
+      <c r="J55" s="21"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
-      <c r="M55" s="43"/>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="53"/>
+    </row>
+    <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="B56" s="2">
-        <v>7075</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>7890</v>
+      </c>
+      <c r="C56" s="2">
+        <v>8290</v>
+      </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="6"/>
+      <c r="F56" s="2"/>
       <c r="G56" s="6"/>
-      <c r="H56" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
-      <c r="M56" s="44"/>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+      <c r="O56" s="54"/>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" s="15"/>
       <c r="B57" s="1"/>
       <c r="C57" s="23"/>
-      <c r="D57" s="14"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="14"/>
       <c r="F57" s="14"/>
       <c r="G57" s="14"/>
       <c r="H57" s="14"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="23"/>
-      <c r="K57" s="27"/>
-      <c r="L57" s="27"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="23"/>
+      <c r="L57" s="37"/>
       <c r="M57" s="27"/>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="B58" s="46"/>
-      <c r="C58" s="46"/>
-      <c r="D58" s="32"/>
+      <c r="N57" s="27"/>
+      <c r="O57" s="27"/>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="56"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="40"/>
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
       <c r="H58" s="32"/>
-      <c r="I58" s="33"/>
-      <c r="J58" s="31"/>
-      <c r="K58" s="32"/>
-      <c r="L58" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="M58" s="47"/>
-    </row>
-    <row r="59" spans="1:13">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="14"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="31"/>
+      <c r="L58" s="31"/>
+      <c r="M58" s="32"/>
+      <c r="N58" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="O58" s="57"/>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" s="47"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="36"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="23"/>
       <c r="L59" s="37"/>
-      <c r="M59" s="37"/>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="14"/>
+      <c r="M59" s="14"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="48"/>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" s="47"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="36"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
       <c r="H60" s="14"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="23"/>
-      <c r="K60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="23"/>
       <c r="L60" s="37"/>
-      <c r="M60" s="37"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="29"/>
+      <c r="M60" s="14"/>
+      <c r="N60" s="48"/>
+      <c r="O60" s="48"/>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="49"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="38"/>
       <c r="E61" s="29"/>
       <c r="F61" s="29"/>
       <c r="G61" s="29"/>
       <c r="H61" s="29"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="29"/>
-      <c r="K61" s="28"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="39"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="29"/>
+      <c r="L61" s="29"/>
+      <c r="M61" s="28"/>
+      <c r="N61" s="50"/>
+      <c r="O61" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="K4:M4"/>
     <mergeCell ref="A59:C60"/>
-    <mergeCell ref="L59:M60"/>
+    <mergeCell ref="N59:O60"/>
     <mergeCell ref="A61:C61"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="H45:M45"/>
-    <mergeCell ref="H46:L46"/>
-    <mergeCell ref="M46:M56"/>
-    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
-    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
02.06.19 Today Last 12:31am Sales Updated
</commit_message>
<xml_diff>
--- a/May/Othes/Allocation Sheet.xlsx
+++ b/May/Othes/Allocation Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="109">
   <si>
     <t>BL60</t>
   </si>
@@ -241,9 +241,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t xml:space="preserve">Tulip-2 </t>
-  </si>
-  <si>
     <t>Distributor Of Symphony (Mobile Hand Set) Edison Group</t>
   </si>
   <si>
@@ -328,10 +325,22 @@
     <t>CP</t>
   </si>
   <si>
-    <t>DSR NAME:   Md Shohel Rana</t>
-  </si>
-  <si>
     <t>Z15</t>
+  </si>
+  <si>
+    <t>DSR NAME:   Md Robiul Islam</t>
+  </si>
+  <si>
+    <t>Tulip-2</t>
+  </si>
+  <si>
+    <t>Robiul: 01751-312831</t>
+  </si>
+  <si>
+    <t>i72</t>
+  </si>
+  <si>
+    <t>Office:01715-116767</t>
   </si>
 </sst>
 </file>
@@ -341,7 +350,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,13 +479,6 @@
     </font>
     <font>
       <b/>
-      <sz val="26"/>
-      <color theme="1"/>
-      <name val="Bauhaus 93"/>
-      <family val="5"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -494,6 +496,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Bauhaus 93"/>
+      <family val="5"/>
     </font>
   </fonts>
   <fills count="4">
@@ -600,7 +616,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -671,7 +687,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -693,7 +709,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -710,8 +726,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -725,9 +759,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,29 +777,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1162,7 +1181,7 @@
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1182,69 +1201,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="32.25" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="57" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+    </row>
+    <row r="3" spans="1:18" s="35" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-    </row>
-    <row r="3" spans="1:18" s="35" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
     </row>
     <row r="4" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+      <c r="A4" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="41"/>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
@@ -1252,12 +1275,12 @@
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="26"/>
-      <c r="L4" s="59" t="s">
+      <c r="L4" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickTop="1">
       <c r="A5" s="11" t="s">
@@ -1267,10 +1290,10 @@
         <v>13</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>7</v>
@@ -1289,10 +1312,10 @@
         <v>13</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M5" s="12" t="s">
         <v>7</v>
@@ -1379,7 +1402,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J8" s="2">
         <v>5750</v>
@@ -1408,7 +1431,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J9" s="4">
         <v>17790</v>
@@ -1437,7 +1460,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J10" s="4">
         <v>10330</v>
@@ -1466,7 +1489,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J11" s="4">
         <v>5570</v>
@@ -1495,7 +1518,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J12" s="4">
         <v>4640</v>
@@ -1510,7 +1533,7 @@
     </row>
     <row r="13" spans="1:18" ht="15.95" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="7">
         <v>900</v>
@@ -1727,7 +1750,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J20" s="4">
         <v>3630</v>
@@ -1785,7 +1808,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J22" s="4">
         <v>3340</v>
@@ -1829,7 +1852,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.95" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24" s="7">
         <v>1290</v>
@@ -1843,7 +1866,7 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J24" s="4">
         <v>5740</v>
@@ -1858,7 +1881,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.95" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" s="7">
         <v>1190</v>
@@ -1872,7 +1895,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J25" s="4">
         <v>4500</v>
@@ -1916,7 +1939,7 @@
     </row>
     <row r="27" spans="1:15" ht="15.95" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" s="7">
         <v>1170</v>
@@ -1930,7 +1953,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J27" s="4">
         <v>4015</v>
@@ -2003,7 +2026,7 @@
     </row>
     <row r="30" spans="1:15" ht="15.95" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" s="7">
         <v>1225</v>
@@ -2104,7 +2127,7 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J33" s="4">
         <v>4220</v>
@@ -2191,7 +2214,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J36" s="4">
         <v>8270</v>
@@ -2206,7 +2229,7 @@
     </row>
     <row r="37" spans="1:15" ht="15.95" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="7">
         <v>1200</v>
@@ -2264,7 +2287,7 @@
     </row>
     <row r="39" spans="1:15" ht="15.95" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" s="7">
         <v>1730</v>
@@ -2307,7 +2330,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J40" s="9">
         <v>8820</v>
@@ -2335,9 +2358,15 @@
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="6"/>
+      <c r="I41" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="J41" s="4">
+        <v>5940</v>
+      </c>
+      <c r="K41" s="6">
+        <v>6390</v>
+      </c>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
@@ -2368,7 +2397,7 @@
     </row>
     <row r="43" spans="1:15" ht="15.95" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" s="7">
         <v>1050</v>
@@ -2404,14 +2433,14 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
-      <c r="I44" s="46" t="s">
+      <c r="I44" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="J44" s="54"/>
+      <c r="J44" s="43"/>
       <c r="K44" s="25"/>
       <c r="L44" s="39"/>
-      <c r="M44" s="46"/>
-      <c r="N44" s="46"/>
+      <c r="M44" s="42"/>
+      <c r="N44" s="42"/>
       <c r="O44" s="17"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -2429,13 +2458,13 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="46"/>
-      <c r="N45" s="46"/>
-      <c r="O45" s="46"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="42"/>
+      <c r="L45" s="42"/>
+      <c r="M45" s="42"/>
+      <c r="N45" s="42"/>
+      <c r="O45" s="42"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -2452,15 +2481,15 @@
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="47" t="s">
+      <c r="I46" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="J46" s="47"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="47"/>
-      <c r="M46" s="47"/>
-      <c r="N46" s="47"/>
-      <c r="O46" s="48"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="52"/>
+      <c r="L46" s="52"/>
+      <c r="M46" s="52"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="53"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -2483,13 +2512,13 @@
       <c r="J47" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K47" s="51" t="s">
+      <c r="K47" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="L47" s="51"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="51"/>
-      <c r="O47" s="49"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="56"/>
+      <c r="N47" s="56"/>
+      <c r="O47" s="54"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="2" t="s">
@@ -2514,7 +2543,7 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
-      <c r="O48" s="49"/>
+      <c r="O48" s="54"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="2" t="s">
@@ -2539,7 +2568,7 @@
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
-      <c r="O49" s="49"/>
+      <c r="O49" s="54"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="3" t="s">
@@ -2564,7 +2593,7 @@
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
-      <c r="O50" s="49"/>
+      <c r="O50" s="54"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="3" t="s">
@@ -2589,7 +2618,7 @@
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
       <c r="N51" s="6"/>
-      <c r="O51" s="49"/>
+      <c r="O51" s="54"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="3" t="s">
@@ -2614,11 +2643,11 @@
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
-      <c r="O52" s="49"/>
+      <c r="O52" s="54"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" s="3">
         <v>5750</v>
@@ -2639,11 +2668,11 @@
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
-      <c r="O53" s="49"/>
+      <c r="O53" s="54"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B54" s="3">
         <v>6540</v>
@@ -2664,11 +2693,11 @@
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
-      <c r="O54" s="49"/>
+      <c r="O54" s="54"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B55" s="3">
         <v>8340</v>
@@ -2689,7 +2718,7 @@
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
-      <c r="O55" s="49"/>
+      <c r="O55" s="54"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="2" t="s">
@@ -2714,7 +2743,7 @@
       <c r="L56" s="6"/>
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
-      <c r="O56" s="50"/>
+      <c r="O56" s="55"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="15"/>
@@ -2734,11 +2763,11 @@
       <c r="O57" s="27"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="52" t="s">
+      <c r="A58" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="52"/>
-      <c r="C58" s="52"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
       <c r="D58" s="40"/>
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
@@ -2749,15 +2778,15 @@
       <c r="K58" s="31"/>
       <c r="L58" s="31"/>
       <c r="M58" s="32"/>
-      <c r="N58" s="53" t="s">
+      <c r="N58" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="O58" s="53"/>
+      <c r="O58" s="58"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="42"/>
-      <c r="B59" s="42"/>
-      <c r="C59" s="42"/>
+      <c r="A59" s="48"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="48"/>
       <c r="D59" s="36"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -2768,13 +2797,13 @@
       <c r="K59" s="23"/>
       <c r="L59" s="37"/>
       <c r="M59" s="14"/>
-      <c r="N59" s="43"/>
-      <c r="O59" s="43"/>
+      <c r="N59" s="49"/>
+      <c r="O59" s="49"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="42"/>
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
+      <c r="A60" s="48"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="48"/>
       <c r="D60" s="36"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -2785,15 +2814,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="37"/>
       <c r="M60" s="14"/>
-      <c r="N60" s="43"/>
-      <c r="O60" s="43"/>
+      <c r="N60" s="49"/>
+      <c r="O60" s="49"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="44" t="s">
+      <c r="A61" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="44"/>
-      <c r="C61" s="44"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="38"/>
       <c r="E61" s="29"/>
       <c r="F61" s="29"/>
@@ -2804,18 +2833,14 @@
       <c r="K61" s="29"/>
       <c r="L61" s="29"/>
       <c r="M61" s="28"/>
-      <c r="N61" s="45"/>
-      <c r="O61" s="45"/>
+      <c r="N61" s="51"/>
+      <c r="O61" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A4:D4"/>
+  <mergeCells count="19">
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A59:C60"/>
     <mergeCell ref="N59:O60"/>
     <mergeCell ref="A61:C61"/>
@@ -2826,6 +2851,12 @@
     <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
03.06.19 Today Sales Updated 12:06 am
</commit_message>
<xml_diff>
--- a/May/Othes/Allocation Sheet.xlsx
+++ b/May/Othes/Allocation Sheet.xlsx
@@ -729,9 +729,51 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,48 +788,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1180,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N61" sqref="A1:O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1201,73 +1201,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="32.25" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="61" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="60" t="s">
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
     </row>
     <row r="3" spans="1:18" s="35" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
     </row>
     <row r="4" spans="1:18" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="41"/>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
@@ -1275,12 +1275,12 @@
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="26"/>
-      <c r="L4" s="46" t="s">
+      <c r="L4" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickTop="1">
       <c r="A5" s="11" t="s">
@@ -2433,14 +2433,14 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
-      <c r="I44" s="42" t="s">
+      <c r="I44" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="J44" s="43"/>
+      <c r="J44" s="57"/>
       <c r="K44" s="25"/>
       <c r="L44" s="39"/>
-      <c r="M44" s="42"/>
-      <c r="N44" s="42"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
       <c r="O44" s="17"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -2458,13 +2458,13 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="42"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="42"/>
-      <c r="N45" s="42"/>
-      <c r="O45" s="42"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -2481,15 +2481,15 @@
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="52" t="s">
+      <c r="I46" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J46" s="52"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="52"/>
-      <c r="M46" s="52"/>
-      <c r="N46" s="52"/>
-      <c r="O46" s="53"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="51"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -2512,13 +2512,13 @@
       <c r="J47" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K47" s="56" t="s">
+      <c r="K47" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
-      <c r="O47" s="54"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="54"/>
+      <c r="N47" s="54"/>
+      <c r="O47" s="52"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="2" t="s">
@@ -2543,7 +2543,7 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
-      <c r="O48" s="54"/>
+      <c r="O48" s="52"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="2" t="s">
@@ -2568,7 +2568,7 @@
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
-      <c r="O49" s="54"/>
+      <c r="O49" s="52"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="3" t="s">
@@ -2593,7 +2593,7 @@
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
-      <c r="O50" s="54"/>
+      <c r="O50" s="52"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="3" t="s">
@@ -2618,7 +2618,7 @@
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
       <c r="N51" s="6"/>
-      <c r="O51" s="54"/>
+      <c r="O51" s="52"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="3" t="s">
@@ -2643,7 +2643,7 @@
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
-      <c r="O52" s="54"/>
+      <c r="O52" s="52"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="3" t="s">
@@ -2668,7 +2668,7 @@
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
-      <c r="O53" s="54"/>
+      <c r="O53" s="52"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="3" t="s">
@@ -2693,7 +2693,7 @@
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
-      <c r="O54" s="54"/>
+      <c r="O54" s="52"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="3" t="s">
@@ -2718,7 +2718,7 @@
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
-      <c r="O55" s="54"/>
+      <c r="O55" s="52"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="2" t="s">
@@ -2743,7 +2743,7 @@
       <c r="L56" s="6"/>
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
-      <c r="O56" s="55"/>
+      <c r="O56" s="53"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="15"/>
@@ -2763,11 +2763,11 @@
       <c r="O57" s="27"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="57" t="s">
+      <c r="A58" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="57"/>
-      <c r="C58" s="57"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="55"/>
       <c r="D58" s="40"/>
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
@@ -2778,15 +2778,15 @@
       <c r="K58" s="31"/>
       <c r="L58" s="31"/>
       <c r="M58" s="32"/>
-      <c r="N58" s="58" t="s">
+      <c r="N58" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="O58" s="58"/>
+      <c r="O58" s="56"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="48"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="48"/>
+      <c r="A59" s="45"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
       <c r="D59" s="36"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -2797,13 +2797,13 @@
       <c r="K59" s="23"/>
       <c r="L59" s="37"/>
       <c r="M59" s="14"/>
-      <c r="N59" s="49"/>
-      <c r="O59" s="49"/>
+      <c r="N59" s="46"/>
+      <c r="O59" s="46"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="48"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="48"/>
+      <c r="A60" s="45"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
       <c r="D60" s="36"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -2814,15 +2814,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="37"/>
       <c r="M60" s="14"/>
-      <c r="N60" s="49"/>
-      <c r="O60" s="49"/>
+      <c r="N60" s="46"/>
+      <c r="O60" s="46"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="50" t="s">
+      <c r="A61" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="47"/>
       <c r="D61" s="38"/>
       <c r="E61" s="29"/>
       <c r="F61" s="29"/>
@@ -2833,16 +2833,11 @@
       <c r="K61" s="29"/>
       <c r="L61" s="29"/>
       <c r="M61" s="28"/>
-      <c r="N61" s="51"/>
-      <c r="O61" s="51"/>
+      <c r="N61" s="48"/>
+      <c r="O61" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A59:C60"/>
-    <mergeCell ref="N59:O60"/>
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="I45:O45"/>
@@ -2851,6 +2846,11 @@
     <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A59:C60"/>
+    <mergeCell ref="N59:O60"/>
     <mergeCell ref="I44:J44"/>
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="A2:O2"/>

</xml_diff>

<commit_message>
04.06.19 Todsy Sales detaisl
</commit_message>
<xml_diff>
--- a/May/Othes/Allocation Sheet.xlsx
+++ b/May/Othes/Allocation Sheet.xlsx
@@ -334,13 +334,13 @@
     <t>Tulip-2</t>
   </si>
   <si>
-    <t>Robiul: 01751-312831</t>
-  </si>
-  <si>
     <t>i72</t>
   </si>
   <si>
     <t>Office:01715-116767</t>
+  </si>
+  <si>
+    <t>Shohel: 01774-585840</t>
   </si>
 </sst>
 </file>
@@ -729,6 +729,36 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -743,36 +773,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1180,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N61" sqref="A1:O61"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection sqref="A1:O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1201,27 +1201,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="32.25" customHeight="1">
-      <c r="A1" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="42" t="s">
+      <c r="A1" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="58" t="s">
@@ -2359,7 +2359,7 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J41" s="4">
         <v>5940</v>
@@ -2433,14 +2433,14 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
-      <c r="I44" s="49" t="s">
+      <c r="I44" s="44" t="s">
         <v>14</v>
       </c>
       <c r="J44" s="57"/>
       <c r="K44" s="25"/>
       <c r="L44" s="39"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="49"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="44"/>
       <c r="O44" s="17"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -2458,13 +2458,13 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="49"/>
-      <c r="K45" s="49"/>
-      <c r="L45" s="49"/>
-      <c r="M45" s="49"/>
-      <c r="N45" s="49"/>
-      <c r="O45" s="49"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+      <c r="M45" s="44"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="44"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -2481,15 +2481,15 @@
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="50" t="s">
+      <c r="I46" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-      <c r="L46" s="50"/>
-      <c r="M46" s="50"/>
-      <c r="N46" s="50"/>
-      <c r="O46" s="51"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="45"/>
+      <c r="L46" s="45"/>
+      <c r="M46" s="45"/>
+      <c r="N46" s="45"/>
+      <c r="O46" s="46"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="2" t="s">
@@ -2512,13 +2512,13 @@
       <c r="J47" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K47" s="54" t="s">
+      <c r="K47" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="L47" s="54"/>
-      <c r="M47" s="54"/>
-      <c r="N47" s="54"/>
-      <c r="O47" s="52"/>
+      <c r="L47" s="49"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="49"/>
+      <c r="O47" s="47"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="2" t="s">
@@ -2543,7 +2543,7 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
-      <c r="O48" s="52"/>
+      <c r="O48" s="47"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="2" t="s">
@@ -2568,7 +2568,7 @@
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
-      <c r="O49" s="52"/>
+      <c r="O49" s="47"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="3" t="s">
@@ -2593,7 +2593,7 @@
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
-      <c r="O50" s="52"/>
+      <c r="O50" s="47"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="3" t="s">
@@ -2618,7 +2618,7 @@
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
       <c r="N51" s="6"/>
-      <c r="O51" s="52"/>
+      <c r="O51" s="47"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="3" t="s">
@@ -2643,7 +2643,7 @@
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
-      <c r="O52" s="52"/>
+      <c r="O52" s="47"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="3" t="s">
@@ -2668,7 +2668,7 @@
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
-      <c r="O53" s="52"/>
+      <c r="O53" s="47"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="3" t="s">
@@ -2693,7 +2693,7 @@
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
-      <c r="O54" s="52"/>
+      <c r="O54" s="47"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="3" t="s">
@@ -2718,7 +2718,7 @@
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
-      <c r="O55" s="52"/>
+      <c r="O55" s="47"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="2" t="s">
@@ -2743,7 +2743,7 @@
       <c r="L56" s="6"/>
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
-      <c r="O56" s="53"/>
+      <c r="O56" s="48"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="15"/>
@@ -2763,11 +2763,11 @@
       <c r="O57" s="27"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="55"/>
-      <c r="C58" s="55"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
       <c r="D58" s="40"/>
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
@@ -2778,15 +2778,15 @@
       <c r="K58" s="31"/>
       <c r="L58" s="31"/>
       <c r="M58" s="32"/>
-      <c r="N58" s="56" t="s">
+      <c r="N58" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="O58" s="56"/>
+      <c r="O58" s="51"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="45"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="45"/>
+      <c r="A59" s="55"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="55"/>
       <c r="D59" s="36"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -2797,13 +2797,13 @@
       <c r="K59" s="23"/>
       <c r="L59" s="37"/>
       <c r="M59" s="14"/>
-      <c r="N59" s="46"/>
-      <c r="O59" s="46"/>
+      <c r="N59" s="56"/>
+      <c r="O59" s="56"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="45"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="45"/>
+      <c r="A60" s="55"/>
+      <c r="B60" s="55"/>
+      <c r="C60" s="55"/>
       <c r="D60" s="36"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -2814,15 +2814,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="37"/>
       <c r="M60" s="14"/>
-      <c r="N60" s="46"/>
-      <c r="O60" s="46"/>
+      <c r="N60" s="56"/>
+      <c r="O60" s="56"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="47" t="s">
+      <c r="A61" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="47"/>
-      <c r="C61" s="47"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="42"/>
       <c r="D61" s="38"/>
       <c r="E61" s="29"/>
       <c r="F61" s="29"/>
@@ -2833,19 +2833,11 @@
       <c r="K61" s="29"/>
       <c r="L61" s="29"/>
       <c r="M61" s="28"/>
-      <c r="N61" s="48"/>
-      <c r="O61" s="48"/>
+      <c r="N61" s="43"/>
+      <c r="O61" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A1:E1"/>
@@ -2857,6 +2849,14 @@
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>